<commit_message>
Automatische test-sync: 2025-06-19 10:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -716,8 +716,72 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-19 09:58:11</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-19 09:58:11</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -737,7 +801,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -755,7 +819,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -778,20 +842,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>Klacht</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B4" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 10:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,8 +780,40 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-19 10:28:10</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -801,7 +833,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -846,7 +878,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 11:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -812,8 +812,40 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-19 10:58:11</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -833,7 +865,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -878,7 +910,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 11:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -844,8 +844,40 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-19 11:28:10</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -865,7 +897,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -910,7 +942,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 12:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,8 +876,48 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je bericht. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 18:00 uur. Op zaterdag zijn we geopend van 10:00 tot 15:00 uur. Op zondag zijn we gesloten. Mocht je verder nog vragen hebben, dan hoor ik graag van je.
+Met vriendelijke groet,
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-19 11:58:12</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -897,7 +937,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -915,7 +955,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -965,6 +1005,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Informatieaanvraag</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 12:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -916,8 +916,40 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-19 12:28:11</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -937,7 +969,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -992,7 +1024,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 13:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -948,8 +948,40 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-19 12:58:10</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -969,7 +1001,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -987,7 +1019,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1047,6 +1079,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 13:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -980,8 +980,40 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-19 13:28:11</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1001,7 +1033,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1046,7 +1078,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 14:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1012,8 +1012,40 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-19 13:58:11</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1033,7 +1065,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1098,7 +1130,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 14:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1044,8 +1044,40 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-19 14:28:10</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1065,7 +1097,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1110,7 +1142,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 15:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1076,8 +1076,40 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-19 14:58:10</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1097,7 +1129,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1142,7 +1174,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 15:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1108,8 +1108,40 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-19 15:28:11</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1129,7 +1161,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1184,7 +1216,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 16:00:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1140,8 +1140,40 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-19 15:58:10</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1161,7 +1193,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1232,17 +1264,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Informatieaanvraag</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Informatieaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 16:30:10
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1172,8 +1172,40 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Bestelling</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-19 16:28:11</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1193,7 +1225,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1254,17 +1286,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:47:21
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1204,8 +1204,40 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-19 16:58:11</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1225,7 +1257,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1280,7 +1312,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:48:21
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1236,8 +1236,104 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Sollicitatie</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:47:20</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Sollicitatie</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:47:21</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:48:20</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1257,7 +1353,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1275,7 +1371,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1312,7 +1408,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -1338,10 +1434,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Sollicitatie</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Informatieaanvraag</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B7" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:49:21
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1332,8 +1332,40 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Offerte-aanvraag</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:49:20</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1353,7 +1385,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1371,7 +1403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1451,6 +1483,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Offerte-aanvraag</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:52:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1428,8 +1428,40 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:52:20</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1449,7 +1481,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1504,7 +1536,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:53:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1460,8 +1460,40 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:53:20</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1481,7 +1513,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1542,7 +1574,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Klacht</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1552,11 +1584,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:55:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1492,8 +1492,72 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:55:20</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:55:21</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1513,7 +1577,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1578,7 +1642,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:56:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1556,8 +1556,40 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:56:20</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1577,7 +1609,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1618,7 +1650,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Afmelding</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1628,11 +1660,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Afmelding</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:57:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1588,8 +1588,40 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:57:20</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1609,7 +1641,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1674,7 +1706,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:58:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1620,8 +1620,40 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Sollicitatie</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:58:20</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1641,7 +1673,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1726,7 +1758,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 17:59:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1652,8 +1652,40 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Offerte-aanvraag</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:59:20</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1673,7 +1705,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G33">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1764,17 +1796,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Informatieaanvraag</t>
+          <t>Offerte-aanvraag</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte-aanvraag</t>
+          <t>Informatieaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 18:00:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$9</f>
+              <f>'Dashboard'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$9</f>
+              <f>'Dashboard'!$B$2:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1684,8 +1684,48 @@
         </is>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Openingstijden</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je bericht. Onze openingstijden zijn van maandag tot en met vrijdag van 09:00 tot 18:00 uur. Op zaterdag zijn we geopend van 10:00 tot 17:00 uur. Op zondag zijn we gesloten.
+Met vriendelijke groet,
+[Naam organisatie]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-06-19 18:00:22</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D33">
+  <conditionalFormatting sqref="D2:D34">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1705,7 +1745,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G33">
+  <conditionalFormatting sqref="G2:G34">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1723,7 +1763,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1823,6 +1863,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Openingstijden</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:04:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1724,8 +1724,48 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Openingstijden</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 18:00 uur. Op zaterdag zijn wij geopend van 10:00 tot 15:00 uur. Voor meer informatie of vragen kunt u altijd contact met ons opnemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:04:27</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D34">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1745,7 +1785,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G34">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1836,7 +1876,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte-aanvraag</t>
+          <t>Openingstijden</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1846,17 +1886,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Informatieaanvraag</t>
+          <t>Offerte-aanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Samenwerking</t>
+          <t>Informatieaanvraag</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1866,7 +1906,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Openingstijden</t>
+          <t>Samenwerking</t>
         </is>
       </c>
       <c r="B10" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:05:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1764,8 +1764,40 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:05:25</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1785,7 +1817,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1830,7 +1862,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:06:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1796,8 +1796,40 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Offerte-aanvraag</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:06:25</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1817,7 +1849,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1908,17 +1940,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Openingstijden</t>
+          <t>Offerte-aanvraag</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte-aanvraag</t>
+          <t>Openingstijden</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:07:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1828,8 +1828,40 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Sollicitatie</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:07:25</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D38">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1849,7 +1881,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G38">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1920,17 +1952,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Sollicitatie</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sollicitatie</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:08:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1860,8 +1860,40 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Klacht</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:08:25</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1881,7 +1913,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1946,7 +1978,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:09:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1892,8 +1892,40 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Afmelding</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:09:25</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1913,7 +1945,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1958,7 +1990,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:44:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$10</f>
+              <f>'Dashboard'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$10</f>
+              <f>'Dashboard'!$B$2:$B$11</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1924,8 +1924,40 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:44:29</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1945,7 +1977,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G41">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1963,7 +1995,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2073,6 +2105,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:45:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$11</f>
+              <f>'Dashboard'!$A$2:$A$12</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$11</f>
+              <f>'Dashboard'!$B$2:$B$12</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1956,8 +1956,40 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:45:25</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D41">
+  <conditionalFormatting sqref="D2:D42">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1977,7 +2009,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G41">
+  <conditionalFormatting sqref="G2:G42">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1995,7 +2027,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2115,6 +2147,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 19:50:30
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -216,12 +216,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$12</f>
+              <f>'Dashboard'!$A$2:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$12</f>
+              <f>'Dashboard'!$B$2:$B$13</f>
             </numRef>
           </val>
         </ser>
@@ -607,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1988,8 +1988,72 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:50:26</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-06-19 19:50:27</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D44">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2009,7 +2073,7 @@
       <formula>"Retour"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G44">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2027,7 +2091,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2090,7 +2154,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bestelling</t>
+          <t>Offerte-aanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2100,7 +2164,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte-aanvraag</t>
+          <t>Bestelling</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2110,7 +2174,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Openingstijden</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2120,17 +2184,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Informatieaanvraag</t>
+          <t>Openingstijden</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Samenwerking</t>
+          <t>Informatieaanvraag</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2140,7 +2204,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Samenwerking</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2150,10 +2214,20 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,8 +679,144 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste,
+Bedankt voor je interesse. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 18:00 uur en op zaterdag van 10:00 tot 16:00 uur. Op zondag zijn wij gesloten. Mocht je verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:12:26</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Factuur verzoek</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Kunt u mij de factuur van mijn laatste bestelling toesturen?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:13:10</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:14:09</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Probleem met inloggen</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Ik kan niet inloggen op mijn account. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:15:14</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -700,7 +836,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -718,7 +854,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -748,6 +884,46 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:16:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -815,8 +815,40 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:16:11</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -836,7 +868,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -854,7 +886,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -924,6 +956,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -847,8 +847,40 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:17:14</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -868,7 +900,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -913,7 +945,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:18:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -879,8 +879,40 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:18:10</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -900,7 +932,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -918,7 +950,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -998,6 +1030,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:19:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -911,8 +911,40 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:19:10</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -932,7 +964,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -983,17 +1015,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1003,7 +1035,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -943,8 +943,40 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:20:13</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -964,7 +996,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1005,17 +1037,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -975,8 +975,40 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:21:17</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -996,7 +1028,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1037,7 +1069,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>Samenwerking / Partnerverzoek</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -1047,11 +1079,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Samenwerking / Partnerverzoek</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1007,8 +1007,40 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sponsoraanvraag</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Zou uw bedrijf bereid zijn om ons sportevenement te sponsoren?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:22:10</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1028,7 +1060,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1073,7 +1105,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:23:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1039,8 +1039,40 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:23:17</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1060,7 +1092,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1121,11 +1153,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1141,7 +1173,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1151,7 +1183,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1161,7 +1193,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1071,8 +1071,40 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:24:10</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1092,7 +1124,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1147,7 +1179,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:25:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,8 +1103,40 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:25:27</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1124,7 +1156,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1142,7 +1174,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1195,7 +1227,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1205,7 +1237,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1229,6 +1261,16 @@
         </is>
       </c>
       <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$9</f>
+              <f>'Dashboard'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$9</f>
+              <f>'Dashboard'!$B$2:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1135,8 +1135,40 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:26:27</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1156,7 +1188,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1174,7 +1206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1227,7 +1259,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1237,7 +1269,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1271,6 +1303,16 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1167,8 +1167,40 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:35:10</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1188,7 +1220,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1233,7 +1265,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1199,8 +1199,40 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Probleem met inloggen</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Ik kan niet inloggen op mijn account. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:36:10</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1220,7 +1252,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1281,7 +1313,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1291,17 +1323,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1311,7 +1343,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1231,8 +1231,40 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:37:13</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1252,7 +1284,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1323,7 +1355,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1333,11 +1365,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -1353,7 +1385,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -1363,7 +1395,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1373,7 +1405,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B10" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1263,8 +1263,40 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Factuur verzoek</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Kunt u mij de factuur van mijn laatste bestelling toesturen?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:38:18</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1284,7 +1316,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1345,7 +1377,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -1355,7 +1387,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1375,17 +1407,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1295,8 +1295,40 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Factuur verzoek</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Kunt u mij de factuur van mijn laatste bestelling toesturen?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:39:10</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1316,7 +1348,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1381,7 +1413,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1327,8 +1327,40 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Sponsoraanvraag</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Zou uw bedrijf bereid zijn om ons sportevenement te sponsoren?</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:40:10</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1348,7 +1380,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1393,7 +1425,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1359,8 +1359,40 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:41:10</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1380,7 +1412,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1451,17 +1483,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1471,7 +1503,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B7" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1391,8 +1391,40 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:42:14</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1412,7 +1444,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1467,7 +1499,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1423,8 +1423,40 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:43:13</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1444,7 +1476,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1489,7 +1521,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:44:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1455,8 +1455,40 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Sponsoraanvraag</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Zou uw bedrijf bereid zijn om ons sportevenement te sponsoren?</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:44:10</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1476,7 +1508,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1521,7 +1553,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1487,8 +1487,40 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:45:10</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1508,7 +1540,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1599,7 +1631,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1609,17 +1641,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Openingstijden / Locatie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Sollicitatie / Vacature</t>
+          <t>Openingstijden / Locatie</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -1629,7 +1661,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Sollicitatie / Vacature</t>
         </is>
       </c>
       <c r="B10" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:46:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1519,8 +1519,40 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Probleem met inloggen</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Ik kan niet inloggen op mijn account. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:46:31</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1540,7 +1572,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1611,7 +1643,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1621,11 +1653,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1551,8 +1551,40 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:47:11</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1572,7 +1604,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1633,11 +1665,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -1653,7 +1685,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:51:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1583,8 +1583,40 @@
         </is>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:51:10</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1604,7 +1636,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G30">
+  <conditionalFormatting sqref="G2:G31">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1695,17 +1727,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 21:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1615,8 +1615,40 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Afmelding nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Graag afmelden voor de nieuwsbrief. Dank u.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-06-19 21:52:10</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1636,7 +1668,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G31">
+  <conditionalFormatting sqref="G2:G32">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1701,7 +1733,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:06:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1647,8 +1647,104 @@
         </is>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:06:32</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:06:33</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:06:33</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D35">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1668,7 +1764,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G32">
+  <conditionalFormatting sqref="G2:G35">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1713,7 +1809,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -1759,7 +1855,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1769,11 +1865,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:07:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -211,12 +211,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$10</f>
+              <f>'Dashboard'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$10</f>
+              <f>'Dashboard'!$B$2:$B$11</f>
             </numRef>
           </val>
         </ser>
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1743,8 +1743,40 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:07:35</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D2:D36">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1764,7 +1796,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G35">
+  <conditionalFormatting sqref="G2:G36">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1782,7 +1814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1835,7 +1867,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1845,7 +1877,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1855,7 +1887,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1889,6 +1921,16 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:08:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1775,8 +1775,40 @@
         </is>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Klacht over levering</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Ik ben niet tevreden over mijn bestelling. Ik hoor graag hoe jullie dit oplossen.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Klacht / Probleem</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:08:10</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D36">
+  <conditionalFormatting sqref="D2:D37">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1796,7 +1828,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G36">
+  <conditionalFormatting sqref="G2:G37">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1871,13 +1903,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1897,7 +1929,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:11:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1807,8 +1807,40 @@
         </is>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:11:13</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D37">
+  <conditionalFormatting sqref="D2:D38">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1828,7 +1860,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G37">
+  <conditionalFormatting sqref="G2:G38">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1899,7 +1931,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1909,11 +1941,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1839,8 +1839,48 @@
         </is>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Hallo, ik zou graag willen weten wat jullie openingstijden zijn. Dank je wel!</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank voor uw interesse. Onze openingstijden zijn maandag t/m vrijdag van 9:00 tot 18:00 uur en zaterdag van 10:00 tot 17:00 uur. Op zondag zijn wij gesloten. Voor verdere vragen staan wij graag tot uw dienst.
+Met vriendelijke groet,
+[Naam bedrijf]</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:12:43</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D38">
+  <conditionalFormatting sqref="D2:D39">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1860,7 +1900,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G38">
+  <conditionalFormatting sqref="G2:G39">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1975,7 +2015,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1879,8 +1879,40 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Sponsoraanvraag</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Zou uw bedrijf bereid zijn om ons sportevenement te sponsoren?</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:22:16</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D39">
+  <conditionalFormatting sqref="D2:D40">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1900,7 +1932,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G39">
+  <conditionalFormatting sqref="G2:G40">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1945,7 +1977,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1911,8 +1911,72 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:29:11</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Sollicitatie marketingfunctie</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Hierbij solliciteer ik voor de functie van marketeer. Zie bijlage voor CV.</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Sollicitatie / Vacature</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:29:12</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D42">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1932,7 +1996,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G40">
+  <conditionalFormatting sqref="G2:G42">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1987,7 +2051,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -2057,7 +2121,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:30:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1975,8 +1975,40 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Factuur verzoek</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Kunt u mij de factuur van mijn laatste bestelling toesturen?</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:30:10</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D43">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1996,7 +2028,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G42">
+  <conditionalFormatting sqref="G2:G43">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2067,7 +2099,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2077,7 +2109,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2091,7 +2123,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2007,8 +2007,40 @@
         </is>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:31:10</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D43">
+  <conditionalFormatting sqref="D2:D44">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2028,7 +2060,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G43">
+  <conditionalFormatting sqref="G2:G44">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2073,7 +2105,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:32:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2039,8 +2039,40 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:32:11</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D44">
+  <conditionalFormatting sqref="D2:D45">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2060,7 +2092,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G44">
+  <conditionalFormatting sqref="G2:G45">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2131,17 +2163,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Klacht / Probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Klacht / Probleem</t>
         </is>
       </c>
       <c r="B6" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2071,8 +2071,40 @@
         </is>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Vragen over samenwerking</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Kunnen we samenwerken aan een nieuw project?</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:33:10</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D45">
+  <conditionalFormatting sqref="D2:D46">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2092,7 +2124,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G45">
+  <conditionalFormatting sqref="G2:G46">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2137,7 +2169,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:34:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2103,8 +2103,40 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Is product X op voorraad?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Ik ben geïnteresseerd in product X. Is dit momenteel op voorraad?</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:34:11</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D46">
+  <conditionalFormatting sqref="D2:D47">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2124,7 +2156,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G46">
+  <conditionalFormatting sqref="G2:G47">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2179,7 +2211,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2135,8 +2135,40 @@
         </is>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Probleem met inloggen</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Ik kan niet inloggen op mijn account. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:35:14</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D47">
+  <conditionalFormatting sqref="D2:D48">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2156,7 +2188,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G47">
+  <conditionalFormatting sqref="G2:G48">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2261,7 +2293,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2167,8 +2167,40 @@
         </is>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Uitnodiging voor netwerkevent</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Graag nodig ik u uit voor ons zakelijke netwerkevent volgende maand.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:36:11</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D48">
+  <conditionalFormatting sqref="D2:D49">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2188,7 +2220,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G48">
+  <conditionalFormatting sqref="G2:G49">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2233,7 +2265,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-06-19 22:37:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-06-19.xlsx
+++ b/logs/mail_log_2025-06-19.xlsx
@@ -602,7 +602,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2199,8 +2199,40 @@
         </is>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Offerte voor zakelijke samenwerking</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Kunt u mij een offerte sturen voor 100 stuks product X?</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2025-06-19 22:37:14</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D49">
+  <conditionalFormatting sqref="D2:D50">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2220,7 +2252,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G49">
+  <conditionalFormatting sqref="G2:G50">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2281,17 +2313,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Afmelding / Nieuwsbrief</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Afmelding / Nieuwsbrief</t>
         </is>
       </c>
       <c r="B5" t="n">

</xml_diff>